<commit_message>
fixed logger when merge data
</commit_message>
<xml_diff>
--- a/resource/testData/combined_data.xlsx
+++ b/resource/testData/combined_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cSharp\Crab-Excel-Data-App\resource\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ACC86FA4-D549-4BEE-8D2E-1F36976DE69A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E2B9B01-979C-4658-B940-6CDA3485549D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16710" yWindow="330" windowWidth="11985" windowHeight="11295" xr2:uid="{7115406A-523E-47B8-B395-7B5FC8ECD37A}"/>
+    <workbookView xWindow="16710" yWindow="330" windowWidth="11985" windowHeight="11295" xr2:uid="{46E2DDFE-BCDB-431B-B0FC-E0C85AAA9976}"/>
   </bookViews>
   <sheets>
     <sheet name="total_data" sheetId="2" r:id="rId1"/>
@@ -686,7 +686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD0FB01-A766-465C-B07A-52FB2CB0C7A4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FD7CA7-92E0-4682-985A-2832CE18D330}">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1133,7 +1133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FADDAC0C-0F24-4EC3-87CD-389A3E07A69A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2453DA23-F926-4905-9BD8-FECCE64575A6}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
pretty for log of merge data
</commit_message>
<xml_diff>
--- a/resource/testData/combined_data.xlsx
+++ b/resource/testData/combined_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cSharp\Crab-Excel-Data-App\resource\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E2B9B01-979C-4658-B940-6CDA3485549D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2860675-B4A6-4027-837A-E4BFF7346D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16710" yWindow="330" windowWidth="11985" windowHeight="11295" xr2:uid="{46E2DDFE-BCDB-431B-B0FC-E0C85AAA9976}"/>
+    <workbookView xWindow="16710" yWindow="330" windowWidth="11985" windowHeight="11295" xr2:uid="{4DE6E0AF-CECD-4FE2-AA63-07FE7770CAD7}"/>
   </bookViews>
   <sheets>
     <sheet name="total_data" sheetId="2" r:id="rId1"/>
@@ -686,7 +686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FD7CA7-92E0-4682-985A-2832CE18D330}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7560DB-11E4-48DB-AC7C-BC26A7A84046}">
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1133,7 +1133,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2453DA23-F926-4905-9BD8-FECCE64575A6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78A0360-BE22-4F02-B804-A11C549E8AF2}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
auto detect starting row
</commit_message>
<xml_diff>
--- a/resource/testData/combined_data.xlsx
+++ b/resource/testData/combined_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cSharp\Crab-Excel-Data-App\resource\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F2860675-B4A6-4027-837A-E4BFF7346D81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8021FCB-FF34-4C41-83F0-DA550BF31C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16710" yWindow="330" windowWidth="11985" windowHeight="11295" xr2:uid="{4DE6E0AF-CECD-4FE2-AA63-07FE7770CAD7}"/>
+    <workbookView xWindow="16710" yWindow="330" windowWidth="11985" windowHeight="11295" xr2:uid="{F7D6EE06-FD09-4836-B5CC-E0F98491F091}"/>
   </bookViews>
   <sheets>
     <sheet name="total_data" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="103">
   <si>
     <t>ID</t>
   </si>
@@ -335,6 +335,15 @@
   </si>
   <si>
     <t>Dan</t>
+  </si>
+  <si>
+    <t>31</t>
+  </si>
+  <si>
+    <t>May</t>
+  </si>
+  <si>
+    <t>Bach</t>
   </si>
 </sst>
 </file>
@@ -686,8 +695,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D7560DB-11E4-48DB-AC7C-BC26A7A84046}">
-  <dimension ref="A1:D31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6DC527-B43A-4AB0-AC6C-1D15A8D7A371}">
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1127,13 +1136,27 @@
         <v>7</v>
       </c>
     </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B78A0360-BE22-4F02-B804-A11C549E8AF2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2993BA-CE96-4F9D-87FE-BF9D80194F42}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
change to save data to excel by value2
</commit_message>
<xml_diff>
--- a/resource/testData/combined_data.xlsx
+++ b/resource/testData/combined_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cSharp\Crab-Excel-Data-App\resource\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8021FCB-FF34-4C41-83F0-DA550BF31C8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{37654C47-0B2D-48B8-8661-425BB8E242D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16710" yWindow="330" windowWidth="11985" windowHeight="11295" xr2:uid="{F7D6EE06-FD09-4836-B5CC-E0F98491F091}"/>
+    <workbookView xWindow="16710" yWindow="330" windowWidth="11985" windowHeight="11295" xr2:uid="{CF71DCD6-106B-425B-91DE-04A85D929C1B}"/>
   </bookViews>
   <sheets>
     <sheet name="total_data" sheetId="2" r:id="rId1"/>
@@ -695,7 +695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE6DC527-B43A-4AB0-AC6C-1D15A8D7A371}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5D2F19-9CA0-447F-B6D9-4133ED7EEBFF}">
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1156,7 +1156,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2993BA-CE96-4F9D-87FE-BF9D80194F42}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CF3544-1208-436A-9772-4D9FFA2067D5}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
impl open containing folder
</commit_message>
<xml_diff>
--- a/resource/testData/combined_data.xlsx
+++ b/resource/testData/combined_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\cSharp\Crab-Excel-Data-App\resource\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37654C47-0B2D-48B8-8661-425BB8E242D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E328614-9082-4A71-ABC4-AF128451C1A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16710" yWindow="330" windowWidth="11985" windowHeight="11295" xr2:uid="{CF71DCD6-106B-425B-91DE-04A85D929C1B}"/>
+    <workbookView xWindow="16710" yWindow="330" windowWidth="11985" windowHeight="11295" xr2:uid="{4B786DA7-3D2F-4AE4-A447-46854B8B7E76}"/>
   </bookViews>
   <sheets>
     <sheet name="total_data" sheetId="2" r:id="rId1"/>
@@ -695,7 +695,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5D2F19-9CA0-447F-B6D9-4133ED7EEBFF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5B1287E-AC66-4F34-9827-017DCBB80E20}">
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1156,7 +1156,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5CF3544-1208-436A-9772-4D9FFA2067D5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8EEA6C0-E581-4A10-A2BC-89266AE32DD8}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>